<commit_message>
make research file into executable speeding up process
</commit_message>
<xml_diff>
--- a/cleaned_financials.xlsx
+++ b/cleaned_financials.xlsx
@@ -2,16 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Charts" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Charts1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Charts2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -27,9 +29,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
       <b val="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,19 +49,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -74,7 +65,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -154,6 +145,39 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10334625" cy="6819900"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
       <row>39</row>
       <rowOff>0</rowOff>
     </from>
@@ -181,7 +205,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -502,28 +526,11 @@
   </sheetPr>
   <dimension ref="A1:P701"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
-  <cols>
-    <col width="15.1796875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="21.54296875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="12.7265625" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="8.90625" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="17.81640625" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="8.6328125" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="9.7265625" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="8.81640625" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="9.81640625" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="7.81640625" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="9.81640625" bestFit="1" customWidth="1" min="12" max="12"/>
-    <col width="10.453125" bestFit="1" customWidth="1" min="13" max="13"/>
-    <col width="13.6328125" bestFit="1" customWidth="1" min="14" max="14"/>
-    <col width="11.6328125" bestFit="1" customWidth="1" min="15" max="15"/>
-    <col width="4.81640625" bestFit="1" customWidth="1" min="16" max="16"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -44048,4 +44055,23 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>